<commit_message>
Updated proper column width in Sources worksheet in iso_iec_80000_quantities_and_units.xslx
</commit_message>
<xml_diff>
--- a/tool-support/quantities_lib_generator/data/iso-iec-80000/iso_iec_80000_quantities_and_units.xlsx
+++ b/tool-support/quantities_lib_generator/data/iso-iec-80000/iso_iec_80000_quantities_and_units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repos_git\SysML-v2-Pilot-Implementation\tool-support\quantities_lib_generator\data\iso-iec-80000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B661A0B-7291-4C7C-8D8D-B719BFBBC87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCA140-E5CF-44B6-874B-7D46AE48D51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{28EA1EC5-1826-4DCF-8BDE-A8FD3446083C}"/>
   </bookViews>
@@ -12851,15 +12851,15 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -13098,8 +13098,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>